<commit_message>
fixed legend text size, comment text bug and created project file
</commit_message>
<xml_diff>
--- a/imgs/project_comments.xlsx
+++ b/imgs/project_comments.xlsx
@@ -16,14 +16,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +40,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +48,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +429,71 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>comment_day</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>comment_floor_id</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>comment_tag</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>241</v>
+      </c>
+      <c r="B2" t="n">
+        <v>93</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>456</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>45028</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>241-93-text</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished integration with excel file
</commit_message>
<xml_diff>
--- a/imgs/project_comments.xlsx
+++ b/imgs/project_comments.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,10 +476,8 @@
       <c r="B2" t="n">
         <v>93</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>456</t>
-        </is>
+      <c r="C2" t="n">
+        <v>456</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>45028</v>
@@ -490,6 +488,28 @@
       <c r="F2" t="inlineStr">
         <is>
           <t>241-93-text</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>190</v>
+      </c>
+      <c r="B3" t="n">
+        <v>119</v>
+      </c>
+      <c r="C3" t="n">
+        <v>456</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>45050</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>190-119-text</t>
         </is>
       </c>
     </row>

</xml_diff>